<commit_message>
Cleaned out old models
</commit_message>
<xml_diff>
--- a/Healthcare/Veeva Systems.xlsx
+++ b/Healthcare/Veeva Systems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/financial-modeling/Healthcare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0DFAFF-0483-564B-BF8F-44D26D03C41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D287AADA-5835-204C-B7F8-632B40D39B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -1388,7 +1388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1466,9 +1466,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1683,12 +1680,6 @@
     <xf numFmtId="10" fontId="20" fillId="9" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="9" fontId="20" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1701,11 +1692,17 @@
     <xf numFmtId="9" fontId="4" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1743,6 +1740,7 @@
       <sheetName val="High Growth"/>
       <sheetName val="GARP"/>
       <sheetName val="Watchlist"/>
+      <sheetName val="Small + Speculative"/>
       <sheetName val="Highest Quality"/>
       <sheetName val="GARP HF Buys"/>
       <sheetName val="Value HF Buys"/>
@@ -1760,7 +1758,7 @@
       <sheetData sheetId="7">
         <row r="8">
           <cell r="C8">
-            <v>4.5080000000000002E-2</v>
+            <v>4.2709999999999998E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -1772,6 +1770,7 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1899,11 +1898,11 @@
     <v>Powered by Refinitiv</v>
     <v>225.48500000000001</v>
     <v>157</v>
-    <v>0.86070000000000002</v>
-    <v>-27.5</v>
-    <v>-0.14165800000000001</v>
-    <v>-0.2</v>
-    <v>-1.1999999999999999E-3</v>
+    <v>0.78459999999999996</v>
+    <v>4.6399999999999997</v>
+    <v>2.6619E-2</v>
+    <v>0.96</v>
+    <v>5.3680000000000004E-3</v>
     <v>USD</v>
     <v>Veeva Systems Inc. is a provider of industry cloud solutions for the global life sciences industry. The Company's offerings span cloud software, data, and business consulting and are designed to meet the needs of its customers and their most strategic business functions from research and development (R&amp;D) to commercialization. The Company's industry cloud solutions for the life sciences industry are grouped into two major product families: Veeva Development Cloud and Veeva Commercial Cloud. Veeva Development Cloud includes application suites for the clinical, regulatory, and safety functions of life sciences companies, all built on its proprietary Veeva Vault platform. Veeva Commercial Cloud includes solutions for the sales, medical affairs, and marketing functions of a life sciences company. Its software offerings include Veeva CRM, Veeva Vault PromoMats, Veeva Vault Medical, and Veeva Crossix. Its data offerings include Veeva OpenData, Veeva Link, and Veeva Compass.</v>
     <v>6744</v>
@@ -1911,25 +1910,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4280 Hacienda Drive, PLEASANTON, CA, 94588 US</v>
-    <v>178.39</v>
+    <v>179.91</v>
     <v>Healthcare Equipment &amp; Supplies</v>
     <v>Stock</v>
-    <v>45240.037502233594</v>
+    <v>45262.03026997656</v>
     <v>0</v>
-    <v>165.33</v>
-    <v>26770025965</v>
+    <v>174.04</v>
+    <v>28749301725</v>
     <v>VEEVA SYSTEMS INC.</v>
     <v>VEEVA SYSTEMS INC.</v>
-    <v>178.39</v>
-    <v>50.2622</v>
-    <v>194.13</v>
-    <v>166.63</v>
-    <v>166.4</v>
+    <v>174.04</v>
+    <v>52.588200000000001</v>
+    <v>174.31</v>
+    <v>178.95</v>
+    <v>179.8</v>
     <v>160655500</v>
     <v>VEEV</v>
     <v>VEEVA SYSTEMS INC. (XNYS:VEEV)</v>
-    <v>4562395</v>
-    <v>881728</v>
+    <v>1339306</v>
+    <v>1272668</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -2094,9 +2093,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq</v>
+      <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -2541,9 +2540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XEY196"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J184" sqref="J184"/>
+      <selection pane="topRight" activeCell="P133" sqref="P133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10247,7 +10246,10 @@
         <f>(O128/N128)-1</f>
         <v>1.5027437870283933E-2</v>
       </c>
-      <c r="P129" s="21"/>
+      <c r="P129" s="21">
+        <f>(P128/O128)-1</f>
+        <v>-3.1070306673746328E-2</v>
+      </c>
       <c r="Q129" s="21">
         <f>(Q128/P128)-1</f>
         <v>1.6786924264379E-2</v>
@@ -15859,8 +15861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146FE8F6-9093-B44F-8ACE-FC5FAB10BAA1}">
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15868,297 +15870,297 @@
     <col min="1" max="16" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="115" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="e" vm="1">
+    <row r="1" spans="1:16" s="118" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="117" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-    </row>
-    <row r="2" spans="1:16" s="115" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+    </row>
+    <row r="2" spans="1:16" s="118" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="117"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
     </row>
     <row r="3" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" cm="1">
+      <c r="A3" s="72" cm="1">
         <f t="array" ref="A3">_FV(A1,"Market cap",TRUE)</f>
-        <v>26770025965</v>
-      </c>
-      <c r="B3" s="74" t="s">
+        <v>28749301725</v>
+      </c>
+      <c r="B3" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="74">
         <f>Financials!O8*0.01</f>
         <v>0.70709999999999995</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="75">
+      <c r="E3" s="74">
         <f>SUM(C11:E11)/3</f>
         <v>0.25154521755725329</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="G3" s="77">
-        <f>SUM(Financials!K129:N129)/4</f>
-        <v>2.0015163693110349E-2</v>
-      </c>
-      <c r="H3" s="76" t="s">
+      <c r="G3" s="76">
+        <f>AVERAGE(Financials!N129:S129)</f>
+        <v>6.9985291516089605E-3</v>
+      </c>
+      <c r="H3" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="I3" s="78">
+      <c r="I3" s="77">
         <f>J15*(1+I7)/(I6-I7)</f>
-        <v>33643942591.501328</v>
-      </c>
-      <c r="J3" s="79" t="s">
+        <v>35969877908.536705</v>
+      </c>
+      <c r="J3" s="78" t="s">
         <v>205</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="46">
         <f>(Financials!O172*-1)/Model!A3</f>
         <v>0</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="47" t="s">
         <v>212</v>
       </c>
       <c r="M3" s="36"/>
-      <c r="N3" s="116" t="s">
+      <c r="N3" s="113" t="s">
         <v>206</v>
       </c>
-      <c r="O3" s="117"/>
+      <c r="O3" s="114"/>
       <c r="P3" s="36"/>
     </row>
     <row r="4" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="80">
+      <c r="A4" s="79">
         <f>Financials!O56-Financials!O96-Financials!O105</f>
         <v>3810234000</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="80" t="s">
         <v>207</v>
       </c>
       <c r="C4" s="38">
         <f>Financials!O17*0.01</f>
         <v>0.17739999999999997</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="80" t="s">
         <v>208</v>
       </c>
       <c r="E4" s="38">
         <f>SUM(C13:E13)/3</f>
         <v>0.17593330803013138</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="81" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="83">
+      <c r="G4" s="82">
         <f>A5*(1+(5*G3))</f>
-        <v>176733230.65349245</v>
-      </c>
-      <c r="H4" s="82" t="s">
+        <v>166277261.00058156</v>
+      </c>
+      <c r="H4" s="81" t="s">
         <v>210</v>
       </c>
       <c r="I4" s="37">
         <f>NPV(I6,F15,G15,H15,I15,(J15+I3))</f>
-        <v>27742725163.370846</v>
-      </c>
-      <c r="J4" s="82" t="s">
+        <v>29785400193.329819</v>
+      </c>
+      <c r="J4" s="81" t="s">
         <v>211</v>
       </c>
-      <c r="K4" s="49" cm="1">
+      <c r="K4" s="48" cm="1">
         <f t="array" ref="K4">_FV(A1,"Change (%)",TRUE)</f>
-        <v>-0.14165800000000001</v>
-      </c>
-      <c r="L4" s="50" t="s">
+        <v>2.6619E-2</v>
+      </c>
+      <c r="L4" s="49" t="s">
         <v>251</v>
       </c>
       <c r="M4" s="36"/>
-      <c r="N4" s="118" t="s">
+      <c r="N4" s="115" t="s">
         <v>213</v>
       </c>
-      <c r="O4" s="119"/>
+      <c r="O4" s="116"/>
       <c r="P4" s="36"/>
     </row>
     <row r="5" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="80" cm="1">
+      <c r="A5" s="79" cm="1">
         <f t="array" ref="A5">_FV(A1,"Shares outstanding",TRUE)</f>
         <v>160655500</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="80" t="s">
         <v>214</v>
       </c>
       <c r="C5" s="38">
         <f>Financials!O34*0.01</f>
         <v>0.24199999999999999</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="83" t="s">
         <v>215</v>
       </c>
       <c r="E5" s="38">
         <f>SUM(C16:E16)/3</f>
         <v>0.22570521968523219</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="81" t="s">
         <v>216</v>
       </c>
-      <c r="G5" s="83">
+      <c r="G5" s="82">
         <f>Financials!O56</f>
         <v>3868739000</v>
       </c>
-      <c r="H5" s="82" t="s">
+      <c r="H5" s="81" t="s">
         <v>217</v>
       </c>
       <c r="I5" s="37">
         <f>I4+G5-G6</f>
-        <v>31552959163.370846</v>
-      </c>
-      <c r="J5" s="82" t="s">
+        <v>33595634193.329819</v>
+      </c>
+      <c r="J5" s="81" t="s">
         <v>218</v>
       </c>
-      <c r="K5" s="85" cm="1">
+      <c r="K5" s="84" cm="1">
         <f t="array" ref="K5">_FV(A1,"Price")</f>
-        <v>166.63</v>
-      </c>
-      <c r="L5" s="86" t="s">
+        <v>178.95</v>
+      </c>
+      <c r="L5" s="85" t="s">
         <v>219</v>
       </c>
       <c r="M5" s="36"/>
-      <c r="N5" s="99" t="s">
+      <c r="N5" s="98" t="s">
         <v>220</v>
       </c>
-      <c r="O5" s="100">
+      <c r="O5" s="99">
         <f>Financials!O20</f>
         <v>0</v>
       </c>
       <c r="P5" s="36"/>
     </row>
     <row r="6" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="87">
+      <c r="A6" s="86">
         <f>O20/F10</f>
-        <v>11.300137596032082</v>
-      </c>
-      <c r="B6" s="81" t="s">
+        <v>12.135627574926129</v>
+      </c>
+      <c r="B6" s="80" t="s">
         <v>221</v>
       </c>
       <c r="C6" s="38">
         <f>Financials!O190</f>
         <v>0.43763579104865408</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="83" t="s">
         <v>200</v>
       </c>
       <c r="E6" s="38">
         <f>Financials!O33/Financials!O126</f>
         <v>0.13007113782716212</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="G6" s="83">
+      <c r="G6" s="82">
         <f>Financials!O96+Financials!O105</f>
         <v>58505000</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="81" t="s">
         <v>223</v>
       </c>
-      <c r="I6" s="49">
+      <c r="I6" s="48">
         <f>N25</f>
-        <v>7.8407087921196522E-2</v>
-      </c>
-      <c r="J6" s="82" t="s">
+        <v>7.4953602972156891E-2</v>
+      </c>
+      <c r="J6" s="81" t="s">
         <v>224</v>
       </c>
       <c r="K6" s="39">
         <f>I5/G4</f>
-        <v>178.53438793994752</v>
-      </c>
-      <c r="L6" s="88" t="s">
+        <v>202.04587200418413</v>
+      </c>
+      <c r="L6" s="87" t="s">
         <v>225</v>
       </c>
       <c r="M6" s="36"/>
-      <c r="N6" s="99" t="s">
+      <c r="N6" s="98" t="s">
         <v>226</v>
       </c>
-      <c r="O6" s="100">
+      <c r="O6" s="99">
         <f>Financials!O96</f>
         <v>10652000</v>
       </c>
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="1:16" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="89">
+      <c r="A7" s="88">
         <f>O20/F12</f>
-        <v>36.372317887228263</v>
-      </c>
-      <c r="B7" s="90" t="s">
+        <v>39.061551256793479</v>
+      </c>
+      <c r="B7" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="91">
+      <c r="C7" s="90">
         <f>F15/O21</f>
-        <v>2.8178956238277209E-2</v>
-      </c>
-      <c r="D7" s="90" t="s">
+        <v>2.6242886423697358E-2</v>
+      </c>
+      <c r="D7" s="89" t="s">
         <v>228</v>
       </c>
-      <c r="E7" s="92">
+      <c r="E7" s="91">
         <f>(Financials!O16*(1-0.25))/(Financials!O126+Financials!O105+Financials!O96)</f>
         <v>7.0510345397502061E-2</v>
       </c>
-      <c r="F7" s="90" t="s">
+      <c r="F7" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="G7" s="93">
+      <c r="G7" s="92">
         <f>(Financials!O96+Financials!O105)/Financials!O126</f>
         <v>1.4088617779086716E-2</v>
       </c>
-      <c r="H7" s="94" t="s">
+      <c r="H7" s="93" t="s">
         <v>229</v>
       </c>
-      <c r="I7" s="95">
+      <c r="I7" s="94">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J7" s="96" t="s">
+      <c r="J7" s="95" t="s">
         <v>230</v>
       </c>
-      <c r="K7" s="97">
+      <c r="K7" s="96">
         <f>K6/K5-1</f>
-        <v>7.1442044889560963E-2</v>
-      </c>
-      <c r="L7" s="98" t="s">
+        <v>0.12906326909295407</v>
+      </c>
+      <c r="L7" s="97" t="s">
         <v>231</v>
       </c>
       <c r="M7" s="36"/>
-      <c r="N7" s="99" t="s">
+      <c r="N7" s="98" t="s">
         <v>232</v>
       </c>
-      <c r="O7" s="100">
+      <c r="O7" s="99">
         <f>Financials!O105</f>
         <v>47853000</v>
       </c>
@@ -16178,467 +16180,467 @@
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
-      <c r="N8" s="101" t="s">
+      <c r="N8" s="100" t="s">
         <v>213</v>
       </c>
-      <c r="O8" s="102">
+      <c r="O8" s="101">
         <f>O5/(O6+O7)</f>
         <v>0</v>
       </c>
       <c r="P8" s="36"/>
     </row>
     <row r="9" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52">
+      <c r="A9" s="50"/>
+      <c r="B9" s="51">
         <v>2020</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="51">
         <v>2021</v>
       </c>
-      <c r="D9" s="52">
+      <c r="D9" s="51">
         <v>2022</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="52">
         <v>2023</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="53">
         <v>2024</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="54">
         <v>2025</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="54">
         <v>2026</v>
       </c>
-      <c r="I9" s="55">
+      <c r="I9" s="54">
         <v>2027</v>
       </c>
-      <c r="J9" s="56">
+      <c r="J9" s="55">
         <v>2028</v>
       </c>
       <c r="K9" s="41"/>
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
-      <c r="N9" s="99" t="s">
+      <c r="N9" s="98" t="s">
         <v>233</v>
       </c>
-      <c r="O9" s="100">
+      <c r="O9" s="99">
         <f>Financials!O25</f>
         <v>-36261000</v>
       </c>
       <c r="P9" s="36"/>
     </row>
     <row r="10" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="57">
         <v>1104081000</v>
       </c>
-      <c r="C10" s="58">
+      <c r="C10" s="57">
         <v>1465069000</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="57">
         <v>1850777000</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="58">
         <v>2155060000</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="57">
         <v>2369000000</v>
       </c>
-      <c r="G10" s="58">
+      <c r="G10" s="57">
         <v>2821000000</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="57">
         <v>3237000000</v>
       </c>
-      <c r="I10" s="58">
+      <c r="I10" s="57">
         <v>3689000000</v>
       </c>
-      <c r="J10" s="59">
+      <c r="J10" s="58">
         <v>4186000000</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="N10" s="99" t="s">
+      <c r="N10" s="98" t="s">
         <v>236</v>
       </c>
-      <c r="O10" s="100">
+      <c r="O10" s="99">
         <f>Financials!O24</f>
         <v>503878000</v>
       </c>
       <c r="P10" s="36"/>
     </row>
     <row r="11" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62">
+      <c r="A11" s="60"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61">
         <f t="shared" ref="C11:J11" si="0">(C10/B10)-1</f>
         <v>0.3269578952993486</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="61">
         <f t="shared" si="0"/>
         <v>0.26326951153836431</v>
       </c>
-      <c r="E11" s="62">
+      <c r="E11" s="61">
         <f t="shared" si="0"/>
         <v>0.16440824583404701</v>
       </c>
-      <c r="F11" s="63">
+      <c r="F11" s="62">
         <f t="shared" si="0"/>
         <v>9.92733380973152E-2</v>
       </c>
-      <c r="G11" s="62">
+      <c r="G11" s="61">
         <f t="shared" si="0"/>
         <v>0.19079780498100463</v>
       </c>
-      <c r="H11" s="62">
+      <c r="H11" s="61">
         <f t="shared" si="0"/>
         <v>0.14746543778801846</v>
       </c>
-      <c r="I11" s="62">
+      <c r="I11" s="61">
         <f t="shared" si="0"/>
         <v>0.13963546493666978</v>
       </c>
-      <c r="J11" s="64">
+      <c r="J11" s="63">
         <f t="shared" si="0"/>
         <v>0.13472485768500952</v>
       </c>
-      <c r="K11" s="64">
+      <c r="K11" s="63">
         <f>SUM(F11:J11)/5</f>
         <v>0.14237938069760353</v>
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
-      <c r="N11" s="99" t="s">
+      <c r="N11" s="98" t="s">
         <v>237</v>
       </c>
-      <c r="O11" s="103">
+      <c r="O11" s="102">
         <f>O9/O10</f>
         <v>-7.1963848391872642E-2</v>
       </c>
       <c r="P11" s="36"/>
     </row>
     <row r="12" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="57">
         <v>301118000</v>
       </c>
-      <c r="C12" s="58">
+      <c r="C12" s="57">
         <v>379998000</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="57">
         <v>427390000</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="57">
         <v>487706000</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="64">
         <v>736000000</v>
       </c>
-      <c r="G12" s="58">
+      <c r="G12" s="57">
         <v>919000000</v>
       </c>
-      <c r="H12" s="58">
+      <c r="H12" s="57">
         <v>1047000000</v>
       </c>
-      <c r="I12" s="58">
+      <c r="I12" s="57">
         <v>1227000000</v>
       </c>
-      <c r="J12" s="59">
+      <c r="J12" s="58">
         <v>1318000000</v>
       </c>
-      <c r="K12" s="66" t="s">
+      <c r="K12" s="65" t="s">
         <v>238</v>
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
-      <c r="N12" s="99" t="s">
+      <c r="N12" s="98" t="s">
         <v>239</v>
       </c>
-      <c r="O12" s="103">
+      <c r="O12" s="102">
         <f>O8*(1-O11)</f>
         <v>0</v>
       </c>
       <c r="P12" s="36"/>
     </row>
     <row r="13" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62">
+      <c r="A13" s="60"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61">
         <f t="shared" ref="C13:J13" si="1">(C12/B12)-1</f>
         <v>0.26195710651638238</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="61">
         <f t="shared" si="1"/>
         <v>0.12471644587603103</v>
       </c>
-      <c r="E13" s="62">
+      <c r="E13" s="61">
         <f t="shared" si="1"/>
         <v>0.1411263716979807</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="62">
         <f t="shared" si="1"/>
         <v>0.50910589576507159</v>
       </c>
-      <c r="G13" s="62">
+      <c r="G13" s="61">
         <f t="shared" si="1"/>
         <v>0.24864130434782616</v>
       </c>
-      <c r="H13" s="62">
+      <c r="H13" s="61">
         <f t="shared" si="1"/>
         <v>0.13928182807399336</v>
       </c>
-      <c r="I13" s="62">
+      <c r="I13" s="61">
         <f t="shared" si="1"/>
         <v>0.17191977077363907</v>
       </c>
-      <c r="J13" s="64">
+      <c r="J13" s="63">
         <f t="shared" si="1"/>
         <v>7.4164629176854069E-2</v>
       </c>
-      <c r="K13" s="64">
+      <c r="K13" s="63">
         <f>SUM(F13:J13)/5</f>
         <v>0.22862268562747684</v>
       </c>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
-      <c r="N13" s="118" t="s">
+      <c r="N13" s="115" t="s">
         <v>240</v>
       </c>
-      <c r="O13" s="119"/>
+      <c r="O13" s="116"/>
       <c r="P13" s="36"/>
     </row>
     <row r="14" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="43">
         <f>B12/B10</f>
         <v>0.27273180138051467</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="43">
         <f t="shared" ref="C14:J14" si="2">C12/C10</f>
         <v>0.25937208418170066</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="43">
         <f t="shared" si="2"/>
         <v>0.23092463327564586</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="43">
         <f t="shared" si="2"/>
         <v>0.22630738819336815</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="44">
         <f t="shared" si="2"/>
         <v>0.31067961165048541</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="43">
         <f t="shared" si="2"/>
         <v>0.32577100319035801</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="43">
         <f t="shared" si="2"/>
         <v>0.32344763670064874</v>
       </c>
-      <c r="I14" s="44">
+      <c r="I14" s="43">
         <f t="shared" si="2"/>
         <v>0.33261046354025481</v>
       </c>
-      <c r="J14" s="46">
+      <c r="J14" s="45">
         <f t="shared" si="2"/>
         <v>0.31485905398948877</v>
       </c>
-      <c r="K14" s="46"/>
+      <c r="K14" s="45"/>
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
-      <c r="N14" s="99" t="s">
+      <c r="N14" s="98" t="s">
         <v>242</v>
       </c>
-      <c r="O14" s="103">
+      <c r="O14" s="102">
         <f>'[1]US Treasury Bonds'!$C$8</f>
-        <v>4.5080000000000002E-2</v>
+        <v>4.2709999999999998E-2</v>
       </c>
       <c r="P14" s="36"/>
     </row>
     <row r="15" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="58">
+      <c r="B15" s="57">
         <v>434262000</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="57">
         <v>551246000</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="57">
         <v>764463000</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="57">
         <v>780470000</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="64">
         <v>756000000</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="57">
         <v>968000000</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="57">
         <v>1100000000</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="57">
         <v>1438000000</v>
       </c>
-      <c r="J15" s="59">
+      <c r="J15" s="58">
         <v>1753000000</v>
       </c>
-      <c r="K15" s="66" t="s">
+      <c r="K15" s="65" t="s">
         <v>241</v>
       </c>
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
-      <c r="N15" s="99" t="s">
+      <c r="N15" s="98" t="s">
         <v>243</v>
       </c>
-      <c r="O15" s="104" cm="1">
+      <c r="O15" s="103" cm="1">
         <f t="array" ref="O15">_FV(A1,"Beta")</f>
-        <v>0.86070000000000002</v>
+        <v>0.78459999999999996</v>
       </c>
       <c r="P15" s="36"/>
     </row>
     <row r="16" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="67"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62">
+      <c r="A16" s="66"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61">
         <f t="shared" ref="C16:J16" si="3">(C15/B15)-1</f>
         <v>0.26938576251203195</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="61">
         <f t="shared" si="3"/>
         <v>0.38679101526360271</v>
       </c>
-      <c r="E16" s="62">
+      <c r="E16" s="61">
         <f t="shared" si="3"/>
         <v>2.0938881280061938E-2</v>
       </c>
-      <c r="F16" s="63">
+      <c r="F16" s="62">
         <f t="shared" si="3"/>
         <v>-3.1352902738093658E-2</v>
       </c>
-      <c r="G16" s="62">
+      <c r="G16" s="61">
         <f t="shared" si="3"/>
         <v>0.28042328042328046</v>
       </c>
-      <c r="H16" s="62">
+      <c r="H16" s="61">
         <f t="shared" si="3"/>
         <v>0.13636363636363646</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="61">
         <f t="shared" si="3"/>
         <v>0.30727272727272736</v>
       </c>
-      <c r="J16" s="64">
+      <c r="J16" s="63">
         <f t="shared" si="3"/>
         <v>0.21905424200278167</v>
       </c>
-      <c r="K16" s="64">
+      <c r="K16" s="63">
         <f>SUM(F16:J16)/5</f>
         <v>0.18235219666486646</v>
       </c>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
-      <c r="N16" s="99" t="s">
+      <c r="N16" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="O16" s="103">
+      <c r="O16" s="102">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="P16" s="36"/>
     </row>
     <row r="17" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="43">
         <f>B15/B10</f>
         <v>0.39332440282914027</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="43">
         <f t="shared" ref="C17:J17" si="4">C15/C10</f>
         <v>0.37625941167276078</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="43">
         <f t="shared" si="4"/>
         <v>0.41304976234305918</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="45">
         <f t="shared" si="4"/>
         <v>0.36215697010756082</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="43">
         <f t="shared" si="4"/>
         <v>0.31912199240185735</v>
       </c>
-      <c r="G17" s="44">
+      <c r="G17" s="43">
         <f t="shared" si="4"/>
         <v>0.34314073023750441</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="43">
         <f t="shared" si="4"/>
         <v>0.33982082174853256</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="43">
         <f t="shared" si="4"/>
         <v>0.38980753591759282</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="45">
         <f t="shared" si="4"/>
         <v>0.4187768752986144</v>
       </c>
-      <c r="K17" s="46"/>
+      <c r="K17" s="45"/>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
-      <c r="N17" s="105" t="s">
+      <c r="N17" s="104" t="s">
         <v>240</v>
       </c>
-      <c r="O17" s="106">
+      <c r="O17" s="105">
         <f>(O14)+((O15)*(O16-O14))</f>
-        <v>7.8578443999999997E-2</v>
+        <v>7.5106134000000005E-2</v>
       </c>
       <c r="P17" s="36"/>
     </row>
     <row r="18" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="67" t="s">
         <v>196</v>
       </c>
-      <c r="B18" s="69">
+      <c r="B18" s="68">
         <v>0.12477418331083885</v>
       </c>
-      <c r="C18" s="69">
+      <c r="C18" s="68">
         <v>0.12163684974659124</v>
       </c>
-      <c r="D18" s="69">
+      <c r="D18" s="68">
         <v>0.12781296091833896</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="68">
         <v>9.1156332103860288E-2</v>
       </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="72"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
-      <c r="N18" s="118" t="s">
+      <c r="N18" s="115" t="s">
         <v>245</v>
       </c>
-      <c r="O18" s="119"/>
+      <c r="O18" s="116"/>
       <c r="P18" s="36"/>
     </row>
     <row r="19" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16655,10 +16657,10 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
-      <c r="N19" s="99" t="s">
+      <c r="N19" s="98" t="s">
         <v>223</v>
       </c>
-      <c r="O19" s="107">
+      <c r="O19" s="106">
         <f>O6+O7</f>
         <v>58505000</v>
       </c>
@@ -16678,12 +16680,12 @@
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
-      <c r="N20" s="99" t="s">
+      <c r="N20" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="O20" s="107" cm="1">
+      <c r="O20" s="106" cm="1">
         <f t="array" ref="O20">_FV(A1,"Market cap",TRUE)</f>
-        <v>26770025965</v>
+        <v>28749301725</v>
       </c>
       <c r="P20" s="36"/>
     </row>
@@ -16693,12 +16695,12 @@
         <v>Healthcare Equipment &amp; Supplies</v>
       </c>
       <c r="B21" s="120"/>
-      <c r="C21" s="121" cm="1">
-        <f t="array" ref="C21">_FV(A1,"Year incorporated",TRUE)</f>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120" cm="1">
+        <f t="array" ref="D21">_FV(A1,"Year incorporated",TRUE)</f>
         <v>2007</v>
       </c>
-      <c r="D21" s="121"/>
-      <c r="E21" s="42"/>
+      <c r="E21" s="120"/>
       <c r="F21" s="41"/>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
@@ -16706,24 +16708,24 @@
       <c r="J21" s="41"/>
       <c r="K21" s="41"/>
       <c r="M21" s="41"/>
-      <c r="N21" s="99" t="s">
+      <c r="N21" s="98" t="s">
         <v>246</v>
       </c>
-      <c r="O21" s="107">
+      <c r="O21" s="106">
         <f>O19+O20</f>
-        <v>26828530965</v>
+        <v>28807806725</v>
       </c>
       <c r="P21" s="36"/>
     </row>
     <row r="22" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="120" t="str" cm="1">
+      <c r="A22" s="119" t="str" cm="1">
         <f t="array" ref="A22">_FV(A1,"Description")</f>
         <v>Veeva Systems Inc. is a provider of industry cloud solutions for the global life sciences industry. The Company's offerings span cloud software, data, and business consulting and are designed to meet the needs of its customers and their most strategic business functions from research and development (R&amp;D) to commercialization. The Company's industry cloud solutions for the life sciences industry are grouped into two major product families: Veeva Development Cloud and Veeva Commercial Cloud. Veeva Development Cloud includes application suites for the clinical, regulatory, and safety functions of life sciences companies, all built on its proprietary Veeva Vault platform. Veeva Commercial Cloud includes solutions for the sales, medical affairs, and marketing functions of a life sciences company. Its software offerings include Veeva CRM, Veeva Vault PromoMats, Veeva Vault Medical, and Veeva Crossix. Its data offerings include Veeva OpenData, Veeva Link, and Veeva Compass.</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
@@ -16732,21 +16734,21 @@
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
-      <c r="N22" s="101" t="s">
+      <c r="N22" s="100" t="s">
         <v>247</v>
       </c>
-      <c r="O22" s="108">
+      <c r="O22" s="107">
         <f>(O19/O21)</f>
-        <v>2.1807008395772595E-3</v>
+        <v>2.0308731087545161E-3</v>
       </c>
       <c r="P22" s="36"/>
     </row>
     <row r="23" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="120"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="120"/>
+      <c r="A23" s="119"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
@@ -16755,21 +16757,21 @@
       <c r="K23" s="41"/>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
-      <c r="N23" s="105" t="s">
+      <c r="N23" s="104" t="s">
         <v>248</v>
       </c>
-      <c r="O23" s="109">
+      <c r="O23" s="108">
         <f>O20/O21</f>
-        <v>0.99781929916042278</v>
+        <v>0.99796912689124551</v>
       </c>
       <c r="P23" s="36"/>
     </row>
     <row r="24" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="120"/>
-      <c r="B24" s="120"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="120"/>
+      <c r="A24" s="119"/>
+      <c r="B24" s="119"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
@@ -16778,18 +16780,18 @@
       <c r="K24" s="41"/>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
-      <c r="N24" s="110" t="s">
+      <c r="N24" s="109" t="s">
         <v>249</v>
       </c>
-      <c r="O24" s="111"/>
+      <c r="O24" s="110"/>
       <c r="P24" s="36"/>
     </row>
     <row r="25" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="120"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
+      <c r="A25" s="119"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
@@ -16798,19 +16800,19 @@
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
-      <c r="N25" s="112">
+      <c r="N25" s="111">
         <f>(O22*O12)+(O23*O17)</f>
-        <v>7.8407087921196522E-2</v>
-      </c>
-      <c r="O25" s="113"/>
+        <v>7.4953602972156891E-2</v>
+      </c>
+      <c r="O25" s="112"/>
       <c r="P25" s="36"/>
     </row>
     <row r="26" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="120"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
+      <c r="A26" s="119"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
@@ -16824,11 +16826,11 @@
       <c r="P26" s="36"/>
     </row>
     <row r="27" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="120"/>
-      <c r="B27" s="120"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
+      <c r="A27" s="119"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="119"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
@@ -16842,11 +16844,11 @@
       <c r="P27" s="36"/>
     </row>
     <row r="28" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="120"/>
-      <c r="B28" s="120"/>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="120"/>
+      <c r="A28" s="119"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="119"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -16860,11 +16862,11 @@
       <c r="P28" s="36"/>
     </row>
     <row r="29" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="120"/>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="120"/>
-      <c r="E29" s="120"/>
+      <c r="A29" s="119"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -16878,11 +16880,11 @@
       <c r="P29" s="36"/>
     </row>
     <row r="30" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="120"/>
-      <c r="B30" s="120"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="120"/>
+      <c r="A30" s="119"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="119"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
@@ -17658,9 +17660,9 @@
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="N18:O18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A22:E30"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" display="https://finbox.com/NYSE:VEEV/explorer/revenue_proj" xr:uid="{DC91032B-6DB2-664F-AE52-DFF87BF6AEA0}"/>

</xml_diff>